<commit_message>
updated link to messy_cirrhosis on README frontpage
</commit_message>
<xml_diff>
--- a/data-raw/messy_data/messy_bp.xlsx
+++ b/data-raw/messy_data/messy_bp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhiggins/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhiggins/Documents/RCode/medicaldata/data-raw/messy_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22DCE52E-733E-AF42-A32A-630745C9892A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45194C74-7853-1D45-97ED-A36C69FD7708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31760" yWindow="12180" windowWidth="29660" windowHeight="17440" xr2:uid="{89F9A108-46D2-2745-BF47-F43D172BAB69}"/>
+    <workbookView xWindow="-31760" yWindow="12400" windowWidth="29660" windowHeight="17440" xr2:uid="{89F9A108-46D2-2745-BF47-F43D172BAB69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="82">
   <si>
     <t>Race</t>
   </si>
@@ -281,15 +281,6 @@
   </si>
   <si>
     <t>152/68</t>
-  </si>
-  <si>
-    <t>superpril</t>
-  </si>
-  <si>
-    <t>wondersaartan</t>
-  </si>
-  <si>
-    <t>Treatment</t>
   </si>
 </sst>
 </file>
@@ -305,7 +296,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,18 +321,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -355,9 +334,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -367,8 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,16 +660,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C4237C-FCA1-E744-908F-B50945A07518}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="14" max="14" width="19.5" customWidth="1"/>
     <col min="15" max="15" width="27.5" customWidth="1"/>
@@ -704,18 +679,18 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="3" t="s">
+      <c r="I3" s="1"/>
+      <c r="J3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="4" t="s">
+      <c r="K3" s="2"/>
+      <c r="L3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="4"/>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -759,7 +734,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
@@ -768,7 +743,7 @@
       <c r="C5">
         <v>30</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>1967</v>
       </c>
       <c r="E5" t="s">
@@ -800,7 +775,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+      <c r="A6">
         <v>2</v>
       </c>
       <c r="B6">
@@ -809,7 +784,7 @@
       <c r="C6">
         <v>12</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>1990</v>
       </c>
       <c r="E6" t="s">
@@ -841,7 +816,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7">
         <v>3</v>
       </c>
       <c r="B7">
@@ -850,7 +825,7 @@
       <c r="C7">
         <v>4</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>1989</v>
       </c>
       <c r="E7" t="s">
@@ -882,8 +857,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>4</v>
+      <c r="A8">
+        <v>3</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -891,7 +866,7 @@
       <c r="C8">
         <v>8</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>1977</v>
       </c>
       <c r="E8" t="s">
@@ -923,8 +898,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>5</v>
+      <c r="A9">
+        <v>4</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -932,7 +907,7 @@
       <c r="C9">
         <v>14</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>1963</v>
       </c>
       <c r="E9" t="s">
@@ -964,8 +939,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>6</v>
+      <c r="A10">
+        <v>5</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -973,7 +948,7 @@
       <c r="C10">
         <v>19</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>1973</v>
       </c>
       <c r="E10" t="s">
@@ -1005,8 +980,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>7</v>
+      <c r="A11">
+        <v>6</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1014,7 +989,7 @@
       <c r="C11">
         <v>23</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="4">
         <v>1986</v>
       </c>
       <c r="E11" t="s">
@@ -1046,8 +1021,8 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>8</v>
+      <c r="A12">
+        <v>7</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -1055,7 +1030,7 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="4">
         <v>1956</v>
       </c>
       <c r="E12" t="s">
@@ -1087,8 +1062,8 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>9</v>
+      <c r="A13">
+        <v>8</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -1096,7 +1071,7 @@
       <c r="C13">
         <v>17</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="4">
         <v>1961</v>
       </c>
       <c r="E13" t="s">
@@ -1128,8 +1103,8 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>10</v>
+      <c r="A14">
+        <v>8</v>
       </c>
       <c r="B14">
         <v>12</v>
@@ -1137,7 +1112,7 @@
       <c r="C14">
         <v>24</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="4">
         <v>1967</v>
       </c>
       <c r="E14" t="s">
@@ -1169,7 +1144,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
+      <c r="A15">
         <v>11</v>
       </c>
       <c r="B15">
@@ -1178,7 +1153,7 @@
       <c r="C15">
         <v>27</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="4">
         <v>1971</v>
       </c>
       <c r="E15" t="s">
@@ -1210,7 +1185,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
+      <c r="A16">
         <v>12</v>
       </c>
       <c r="B16">
@@ -1219,7 +1194,7 @@
       <c r="C16">
         <v>16</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="4">
         <v>1970</v>
       </c>
       <c r="E16" t="s">
@@ -1251,7 +1226,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
+      <c r="A17">
         <v>13</v>
       </c>
       <c r="B17">
@@ -1260,7 +1235,7 @@
       <c r="C17">
         <v>18</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="4">
         <v>1963</v>
       </c>
       <c r="E17" t="s">
@@ -1292,7 +1267,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
+      <c r="A18">
         <v>14</v>
       </c>
       <c r="B18">
@@ -1301,7 +1276,7 @@
       <c r="C18">
         <v>3</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="4">
         <v>1989</v>
       </c>
       <c r="E18" t="s">
@@ -1333,7 +1308,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
+      <c r="A19">
         <v>15</v>
       </c>
       <c r="B19">
@@ -1342,7 +1317,7 @@
       <c r="C19">
         <v>8</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="4">
         <v>1990</v>
       </c>
       <c r="E19" t="s">
@@ -1374,7 +1349,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
+      <c r="A20">
         <v>16</v>
       </c>
       <c r="B20">
@@ -1383,7 +1358,7 @@
       <c r="C20">
         <v>13</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="4">
         <v>1987</v>
       </c>
       <c r="E20" t="s">
@@ -1415,7 +1390,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
+      <c r="A21">
         <v>17</v>
       </c>
       <c r="B21">
@@ -1424,7 +1399,7 @@
       <c r="C21">
         <v>27</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="4">
         <v>1980</v>
       </c>
       <c r="E21" t="s">
@@ -1456,8 +1431,8 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
-        <v>18</v>
+      <c r="A22">
+        <v>19</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -1465,7 +1440,7 @@
       <c r="C22">
         <v>11</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="4">
         <v>1975</v>
       </c>
       <c r="E22" t="s">
@@ -1497,8 +1472,8 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="5">
-        <v>19</v>
+      <c r="A23">
+        <v>20</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1506,7 +1481,7 @@
       <c r="C23">
         <v>7</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="4">
         <v>1967</v>
       </c>
       <c r="E23" t="s">
@@ -1538,8 +1513,8 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="6">
-        <v>20</v>
+      <c r="A24">
+        <v>21</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1547,7 +1522,7 @@
       <c r="C24">
         <v>9</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="4">
         <v>1988</v>
       </c>
       <c r="E24" t="s">
@@ -1576,21 +1551,6 @@
       </c>
       <c r="M24">
         <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>